<commit_message>
Add Script sheet to input .xlsx
</commit_message>
<xml_diff>
--- a/DSbulkUploadR_input.xlsx
+++ b/DSbulkUploadR_input.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlbaker\Rdev_local\DSbulkUploadR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AC854D-C5C3-4179-B048-A69EDE6C539D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA72FB1E-6F1C-47E3-BD7F-6D4702284AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29580" yWindow="450" windowWidth="21345" windowHeight="13275" activeTab="1" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
+    <workbookView xWindow="33180" yWindow="1410" windowWidth="24615" windowHeight="13275" activeTab="1" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
   </bookViews>
   <sheets>
     <sheet name="GenericDataset" sheetId="4" r:id="rId1"/>
-    <sheet name="GenericDocument" sheetId="2" r:id="rId2"/>
-    <sheet name="AudioRecording" sheetId="1" r:id="rId3"/>
-    <sheet name="WebSite" sheetId="3" r:id="rId4"/>
-    <sheet name="Project" sheetId="5" r:id="rId5"/>
+    <sheet name="FieldNotes" sheetId="6" r:id="rId2"/>
+    <sheet name="GenericDocument" sheetId="2" r:id="rId3"/>
+    <sheet name="AudioRecording" sheetId="1" r:id="rId4"/>
+    <sheet name="WebSite" sheetId="3" r:id="rId5"/>
+    <sheet name="Project" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="76">
   <si>
     <t>reference_type</t>
   </si>
@@ -243,43 +244,31 @@
     <t>Project</t>
   </si>
   <si>
+    <t>stewards_email_list</t>
+  </si>
+  <si>
     <t>leads_email_list</t>
   </si>
   <si>
-    <t>test project1</t>
-  </si>
-  <si>
-    <t>really just testing things out</t>
-  </si>
-  <si>
-    <t>Nothing of note</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>one, keyword, at, a, time</t>
-  </si>
-  <si>
-    <t>test project2</t>
-  </si>
-  <si>
-    <t>Nothing but another test</t>
-  </si>
-  <si>
-    <t>Nothing noteworthy</t>
-  </si>
-  <si>
-    <t>General Privacy</t>
-  </si>
-  <si>
-    <t>john doe</t>
-  </si>
-  <si>
-    <t>john_doe@nps.gov</t>
-  </si>
-  <si>
-    <t>multi-part keyword, please</t>
+    <t>sponsors_email_list</t>
+  </si>
+  <si>
+    <t>FieldNotes</t>
+  </si>
+  <si>
+    <t>YeS</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Test FieldNotes1</t>
+  </si>
+  <si>
+    <t>Test FieldNotes2</t>
+  </si>
+  <si>
+    <t>Test FieldNotes3</t>
   </si>
 </sst>
 </file>
@@ -666,7 +655,7 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -814,11 +803,278 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02740E3C-2CB5-4540-B9FC-9B8FBF6E48A3}">
+  <dimension ref="A1:S4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44975</v>
+      </c>
+      <c r="F2" s="1">
+        <v>45558</v>
+      </c>
+      <c r="G2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S2" s="2">
+        <v>2316278</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="1">
+        <v>44975</v>
+      </c>
+      <c r="F3" s="1">
+        <v>45558</v>
+      </c>
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3" t="s">
+        <v>51</v>
+      </c>
+      <c r="P3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>24</v>
+      </c>
+      <c r="R3" t="s">
+        <v>25</v>
+      </c>
+      <c r="S3" s="2">
+        <v>2316278</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="1">
+        <v>44975</v>
+      </c>
+      <c r="F4" s="1">
+        <v>45558</v>
+      </c>
+      <c r="G4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" t="s">
+        <v>58</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" t="s">
+        <v>51</v>
+      </c>
+      <c r="P4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>24</v>
+      </c>
+      <c r="R4" t="s">
+        <v>25</v>
+      </c>
+      <c r="S4" s="2">
+        <v>2316278</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{D25A4B78-251F-4041-A15B-308ADE4ACC73}">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:F1" xr:uid="{3FFDB4EB-46D3-48E3-BFAF-C9F84595E7CE}">
+      <formula1>18264</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A4" xr:uid="{4C1E8518-3C7F-4113-8E0E-15FBD22F16CE}">
+      <formula1>"FieldNotes"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="S2" r:id="rId1" display="https://irmadev.nps.gov/DataStore/Reference/Profile/2316278" xr:uid="{EFE6BEA7-AC59-4932-9308-09E15F3E8D98}"/>
+    <hyperlink ref="S3" r:id="rId2" display="https://irmadev.nps.gov/DataStore/Reference/Profile/2316278" xr:uid="{FE293882-303B-46B2-9CFA-9BDFA19FC601}"/>
+    <hyperlink ref="S4" r:id="rId3" display="https://irmadev.nps.gov/DataStore/Reference/Profile/2316278" xr:uid="{2B6F997D-5186-4194-8C1E-135B7FE53F5B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C372F4-B2F9-43E8-90EB-ACDD3F5DA605}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -943,7 +1199,7 @@
         <v>25</v>
       </c>
       <c r="S2">
-        <v>2316278</v>
+        <v>2315517</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
@@ -963,7 +1219,7 @@
         <v>45636</v>
       </c>
       <c r="F3" s="1">
-        <v>45639</v>
+        <v>45635</v>
       </c>
       <c r="G3" t="s">
         <v>33</v>
@@ -981,7 +1237,7 @@
         <v>58</v>
       </c>
       <c r="L3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M3" t="s">
         <v>46</v>
@@ -1024,7 +1280,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA704E2-EB95-4E4A-95B2-36E8F6DDD1DD}">
   <dimension ref="A1:T3"/>
   <sheetViews>
@@ -1251,7 +1507,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0591C5C5-FA56-4654-9944-818D77B92433}">
   <dimension ref="A1:S3"/>
   <sheetViews>
@@ -1463,153 +1719,89 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F8CC3E-9092-4E88-8E6A-27D4AA288ABA}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="16.77734375" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" t="s">
         <v>67</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" t="s">
         <v>57</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>45</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>50</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>49</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>66</v>
       </c>
-      <c r="B2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="1">
-        <v>45347</v>
-      </c>
-      <c r="D2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" t="s">
-        <v>71</v>
-      </c>
-      <c r="K2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" t="s">
-        <v>31</v>
-      </c>
-      <c r="N2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="1">
-        <v>45515</v>
-      </c>
-      <c r="D3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-      <c r="I3" t="s">
-        <v>76</v>
-      </c>
-      <c r="J3" t="s">
-        <v>77</v>
-      </c>
-      <c r="K3" t="s">
-        <v>78</v>
-      </c>
-      <c r="L3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M3" t="s">
-        <v>24</v>
-      </c>
-      <c r="N3" t="s">
-        <v>79</v>
-      </c>
     </row>
   </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2" xr:uid="{EB211272-910D-4987-85E2-04583C1EE0CB}">
+      <formula1>"Project"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{4F6100E9-CD6E-492E-841E-2836B1C34381}">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1" xr:uid="{8E582D2C-63A3-4AB1-BD31-039C1F749E66}">
+      <formula1>18264</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
begin support for Script reference type.
</commit_message>
<xml_diff>
--- a/DSbulkUploadR_input.xlsx
+++ b/DSbulkUploadR_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlbaker\Rdev_local\DSbulkUploadR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA72FB1E-6F1C-47E3-BD7F-6D4702284AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A84F0A-D2B6-4E9D-B9A4-E5E7355D5140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33180" yWindow="1410" windowWidth="24615" windowHeight="13275" activeTab="1" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
+    <workbookView xWindow="29580" yWindow="2205" windowWidth="24615" windowHeight="13275" activeTab="2" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
   </bookViews>
   <sheets>
     <sheet name="GenericDataset" sheetId="4" r:id="rId1"/>
@@ -806,11 +806,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02740E3C-2CB5-4540-B9FC-9B8FBF6E48A3}">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="13.88671875" customWidth="1"/>
+    <col min="6" max="6" width="18.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1073,13 +1077,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C372F4-B2F9-43E8-90EB-ACDD3F5DA605}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" customWidth="1"/>
     <col min="11" max="11" width="11.6640625" customWidth="1"/>
     <col min="14" max="14" width="10.6640625" customWidth="1"/>
   </cols>
@@ -1199,7 +1204,7 @@
         <v>25</v>
       </c>
       <c r="S2">
-        <v>2315517</v>
+        <v>2303363</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
@@ -1219,7 +1224,7 @@
         <v>45636</v>
       </c>
       <c r="F3" s="1">
-        <v>45635</v>
+        <v>45637</v>
       </c>
       <c r="G3" t="s">
         <v>33</v>
@@ -1240,7 +1245,7 @@
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N3" t="s">
         <v>48</v>
@@ -1258,7 +1263,7 @@
         <v>32</v>
       </c>
       <c r="S3">
-        <v>2315517</v>
+        <v>2303363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add version number to development heading
</commit_message>
<xml_diff>
--- a/DSbulkUploadR_input.xlsx
+++ b/DSbulkUploadR_input.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlbaker\Rdev_local\DSbulkUploadR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A84F0A-D2B6-4E9D-B9A4-E5E7355D5140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541DBC71-9806-4048-A0D3-6BC6107F91C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29580" yWindow="2205" windowWidth="24615" windowHeight="13275" activeTab="2" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
+    <workbookView xWindow="29280" yWindow="480" windowWidth="24615" windowHeight="13275" activeTab="5" xr2:uid="{8A6EE447-C162-4970-95C2-F79FBBAD4C55}"/>
   </bookViews>
   <sheets>
-    <sheet name="GenericDataset" sheetId="4" r:id="rId1"/>
-    <sheet name="FieldNotes" sheetId="6" r:id="rId2"/>
-    <sheet name="GenericDocument" sheetId="2" r:id="rId3"/>
-    <sheet name="AudioRecording" sheetId="1" r:id="rId4"/>
-    <sheet name="WebSite" sheetId="3" r:id="rId5"/>
-    <sheet name="Project" sheetId="5" r:id="rId6"/>
+    <sheet name="Project" sheetId="5" r:id="rId1"/>
+    <sheet name="GenericDataset" sheetId="4" r:id="rId2"/>
+    <sheet name="FieldNotes" sheetId="6" r:id="rId3"/>
+    <sheet name="GenericDocument" sheetId="2" r:id="rId4"/>
+    <sheet name="AudioRecording" sheetId="1" r:id="rId5"/>
+    <sheet name="Script" sheetId="7" r:id="rId6"/>
+    <sheet name="WebSite" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="85">
   <si>
     <t>reference_type</t>
   </si>
@@ -269,6 +270,33 @@
   </si>
   <si>
     <t>Test FieldNotes3</t>
+  </si>
+  <si>
+    <t>Script</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>scripting_language</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>python</t>
+  </si>
+  <si>
+    <t>0.0.1</t>
+  </si>
+  <si>
+    <t>1.1.0</t>
+  </si>
+  <si>
+    <t>steward_email</t>
+  </si>
+  <si>
+    <t>Data Monkey</t>
   </si>
 </sst>
 </file>
@@ -651,6 +679,99 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F8CC3E-9092-4E88-8E6A-27D4AA288ABA}">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44470</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2" xr:uid="{EB211272-910D-4987-85E2-04583C1EE0CB}">
+      <formula1>"Project"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{4F6100E9-CD6E-492E-841E-2836B1C34381}">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1" xr:uid="{8E582D2C-63A3-4AB1-BD31-039C1F749E66}">
+      <formula1>18264</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B81407D-D8D8-4DE4-AB2A-A11A6520C285}">
   <dimension ref="A1:S2"/>
   <sheetViews>
@@ -802,19 +923,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02740E3C-2CB5-4540-B9FC-9B8FBF6E48A3}">
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="5" max="5" width="13.88671875" customWidth="1"/>
-    <col min="6" max="6" width="18.77734375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -930,8 +1047,8 @@
       <c r="R2" t="s">
         <v>25</v>
       </c>
-      <c r="S2" s="2">
-        <v>2316278</v>
+      <c r="S2">
+        <v>2315517</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
@@ -989,8 +1106,8 @@
       <c r="R3" t="s">
         <v>25</v>
       </c>
-      <c r="S3" s="2">
-        <v>2316278</v>
+      <c r="S3">
+        <v>2315517</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
@@ -1048,8 +1165,8 @@
       <c r="R4" t="s">
         <v>25</v>
       </c>
-      <c r="S4" s="2">
-        <v>2316278</v>
+      <c r="S4">
+        <v>2315517</v>
       </c>
     </row>
   </sheetData>
@@ -1064,27 +1181,21 @@
       <formula1>"FieldNotes"</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="S2" r:id="rId1" display="https://irmadev.nps.gov/DataStore/Reference/Profile/2316278" xr:uid="{EFE6BEA7-AC59-4932-9308-09E15F3E8D98}"/>
-    <hyperlink ref="S3" r:id="rId2" display="https://irmadev.nps.gov/DataStore/Reference/Profile/2316278" xr:uid="{FE293882-303B-46B2-9CFA-9BDFA19FC601}"/>
-    <hyperlink ref="S4" r:id="rId3" display="https://irmadev.nps.gov/DataStore/Reference/Profile/2316278" xr:uid="{2B6F997D-5186-4194-8C1E-135B7FE53F5B}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C372F4-B2F9-43E8-90EB-ACDD3F5DA605}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="17.33203125" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" customWidth="1"/>
+    <col min="5" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.6640625" customWidth="1"/>
     <col min="14" max="14" width="10.6640625" customWidth="1"/>
   </cols>
@@ -1204,7 +1315,7 @@
         <v>25</v>
       </c>
       <c r="S2">
-        <v>2303363</v>
+        <v>2315517</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
@@ -1224,7 +1335,7 @@
         <v>45636</v>
       </c>
       <c r="F3" s="1">
-        <v>45637</v>
+        <v>45635</v>
       </c>
       <c r="G3" t="s">
         <v>33</v>
@@ -1245,7 +1356,7 @@
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="N3" t="s">
         <v>48</v>
@@ -1263,7 +1374,7 @@
         <v>32</v>
       </c>
       <c r="S3">
-        <v>2303363</v>
+        <v>2315517</v>
       </c>
     </row>
   </sheetData>
@@ -1285,7 +1396,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA704E2-EB95-4E4A-95B2-36E8F6DDD1DD}">
   <dimension ref="A1:T3"/>
   <sheetViews>
@@ -1512,7 +1623,222 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D704E2B-E668-4D16-AAE0-B58A99B5B51C}">
+  <dimension ref="A1:T3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2">
+        <v>2303363</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O3" t="s">
+        <v>84</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3">
+        <v>2303363</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C3" xr:uid="{0E11573E-BFDF-4090-ADE3-ACEE7B1130EA}">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{3C490254-272D-499A-BB89-7E62B524A514}">
+      <formula1>"Script"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="P3" r:id="rId1" display="mailto:NRSS_DataStore@nps.gov" xr:uid="{B81D948F-3067-40F8-99D2-80172FE813C2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0591C5C5-FA56-4654-9944-818D77B92433}">
   <dimension ref="A1:S3"/>
   <sheetViews>
@@ -1722,91 +2048,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F8CC3E-9092-4E88-8E6A-27D4AA288ABA}">
-  <dimension ref="A1:R2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I1" t="s">
-        <v>67</v>
-      </c>
-      <c r="J1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>45</v>
-      </c>
-      <c r="N1" t="s">
-        <v>50</v>
-      </c>
-      <c r="O1" t="s">
-        <v>49</v>
-      </c>
-      <c r="P1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2" xr:uid="{EB211272-910D-4987-85E2-04583C1EE0CB}">
-      <formula1>"Project"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{4F6100E9-CD6E-492E-841E-2836B1C34381}">
-      <formula1>"Yes, No"</formula1>
-    </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1" xr:uid="{8E582D2C-63A3-4AB1-BD31-039C1F749E66}">
-      <formula1>18264</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>